<commit_message>
Update: erzeugung dynamischer Komponenten
</commit_message>
<xml_diff>
--- a/src/parsers/PyPSA2PowerSystems/Zuordnung_PyPSA_PowerSytsems.xlsx
+++ b/src/parsers/PyPSA2PowerSystems/Zuordnung_PyPSA_PowerSytsems.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ec488eecafcfc261/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ec488eecafcfc261/Masterarbeit/PowerSystems.jl/src/parsers/PyPSA2PowerSystems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0962E557-B791-4566-AE6E-0E91B0186060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{0962E557-B791-4566-AE6E-0E91B0186060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{193CAC24-4260-4AAB-A270-47C1CB4C1DF6}"/>
   <bookViews>
     <workbookView xWindow="1800" yWindow="1800" windowWidth="14400" windowHeight="7290" xr2:uid="{4BFB8596-127E-4A7E-8332-00D9FF0CB3CF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
   <si>
     <t>PyPSA</t>
   </si>
@@ -157,13 +157,19 @@
   </si>
   <si>
     <t>RESIDUAL_FUEL_OIL</t>
+  </si>
+  <si>
+    <t>Nomenklatur:</t>
+  </si>
+  <si>
+    <t>Technologie_Knoten</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,16 +177,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -203,21 +241,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -533,276 +604,283 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD80FBA9-B4D8-4896-9E6A-3C7668628AE7}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.58984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.58984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A2" s="4" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A3" s="4" t="s">
+      <c r="G2" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A4" s="4" t="s">
+      <c r="G3" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A6" s="4" t="s">
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A10" s="4" t="s">
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A15" s="4" t="s">
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A16" s="4" t="s">
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Nomenklatur angepasst, add dyn comp. alle typen
</commit_message>
<xml_diff>
--- a/src/parsers/PyPSA2PowerSystems/Zuordnung_PyPSA_PowerSytsems.xlsx
+++ b/src/parsers/PyPSA2PowerSystems/Zuordnung_PyPSA_PowerSytsems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ec488eecafcfc261/Masterarbeit/PowerSystems.jl/src/parsers/PyPSA2PowerSystems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{0962E557-B791-4566-AE6E-0E91B0186060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{193CAC24-4260-4AAB-A270-47C1CB4C1DF6}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{0962E557-B791-4566-AE6E-0E91B0186060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C502A867-BCA0-4B0C-A97D-584188F2176D}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1800" windowWidth="14400" windowHeight="7290" xr2:uid="{4BFB8596-127E-4A7E-8332-00D9FF0CB3CF}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{4BFB8596-127E-4A7E-8332-00D9FF0CB3CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
   <si>
     <t>PyPSA</t>
   </si>
@@ -162,7 +162,19 @@
     <t>Nomenklatur:</t>
   </si>
   <si>
-    <t>Technologie_Knoten</t>
+    <t>Bus_Technology_Number</t>
+  </si>
+  <si>
+    <t>Bus:</t>
+  </si>
+  <si>
+    <t>5 Ziffern</t>
+  </si>
+  <si>
+    <t>Number:</t>
+  </si>
+  <si>
+    <t>2 Ziffern</t>
   </si>
 </sst>
 </file>
@@ -254,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -287,6 +299,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -604,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD80FBA9-B4D8-4896-9E6A-3C7668628AE7}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -620,18 +633,18 @@
     <col min="6" max="16384" width="10.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -651,7 +664,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -671,7 +684,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -688,7 +701,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -702,8 +715,14 @@
         <v>33</v>
       </c>
       <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="G5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -719,8 +738,14 @@
       <c r="E6" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="G6" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -737,7 +762,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -754,7 +779,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A9" s="9" t="s">
         <v>13</v>
       </c>
@@ -769,7 +794,7 @@
       </c>
       <c r="E9" s="10"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -786,7 +811,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -803,7 +828,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
@@ -820,7 +845,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
@@ -837,7 +862,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -852,7 +877,7 @@
       </c>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
@@ -867,7 +892,7 @@
       </c>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>

</xml_diff>